<commit_message>
starting optimization created title and description with relevant keywords
</commit_message>
<xml_diff>
--- a/report/Modèle-audit-SEO.xlsx
+++ b/report/Modèle-audit-SEO.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="78">
   <si>
     <t xml:space="preserve">Catégorie</t>
   </si>
@@ -276,6 +276,24 @@
   </si>
   <si>
     <t xml:space="preserve">Dépend surtout de la qualité et du nombre de liens qui pointent vers votre site</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Un lien est de bonne qualité s’il: 1- Provient d’un site connu ou de qualité   2- Se trouve dans un contenu cohérent par rapport à votre domaine métier     3 – Amène un vrai trafic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Google Analytics / Google Search Console</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Permet de savoir tout sur vos visiteurs et les informations détaillées sur les mots clés utilisés et leur position</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comparaison des canaux d’acquisition. Créer des annotation sur Analytics à chque modificcation importance ou ajout de contenu. Permet quelques mois plus tard de voir l’impact des modifications sur votre trafic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">autres données importantes </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> taux de visiteurs récurrents, taux de conversion, taux de rebond, configuration matérielle utilisée</t>
   </si>
 </sst>
 </file>
@@ -402,7 +420,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -469,6 +487,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -550,8 +572,8 @@
   </sheetPr>
   <dimension ref="A1:Z1004"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C58" activeCellId="0" sqref="C58"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C62" activeCellId="0" sqref="C62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.32421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -959,10 +981,30 @@
       <c r="C58" s="2" t="s">
         <v>71</v>
       </c>
+      <c r="D58" s="17" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="60" s="14" customFormat="true" ht="36.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B60" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="C60" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="D60" s="14" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C61" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
added .htaccess + updated report
</commit_message>
<xml_diff>
--- a/report/Modèle-audit-SEO.xlsx
+++ b/report/Modèle-audit-SEO.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="91">
   <si>
     <t xml:space="preserve">Catégorie</t>
   </si>
@@ -56,6 +56,9 @@
   </si>
   <si>
     <t xml:space="preserve">version principale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Title 70 char max contain relevant keywords</t>
   </si>
   <si>
     <t xml:space="preserve">pas de contenu dupliqué</t>
@@ -97,6 +100,7 @@
         <color rgb="FFFFFFFF"/>
         <rFont val="Arial"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Document doesn't use</t>
     </r>
@@ -105,6 +109,7 @@
         <sz val="12"/>
         <rFont val="Arial"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> legible font sizes</t>
     </r>
@@ -238,6 +243,7 @@
         <sz val="12"/>
         <rFont val="Arial"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Permettent j’ajouter des résultats enrichis (cf screen ) </t>
     </r>
@@ -247,6 +253,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Arial"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">faire screen </t>
     </r>
@@ -255,6 +262,7 @@
         <sz val="12"/>
         <rFont val="Arial"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">==&gt; attirent l’oeil diu visiteur</t>
     </r>
@@ -294,6 +302,42 @@
   </si>
   <si>
     <t xml:space="preserve"> taux de visiteurs récurrents, taux de conversion, taux de rebond, configuration matérielle utilisée</t>
+  </si>
+  <si>
+    <t xml:space="preserve">relevant text placed in img (=&gt;not indexed)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OPTIMIZATION / PERFORMANCE ( cf lighthouse pre-optimization report)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">compression des images</t>
+  </si>
+  <si>
+    <t xml:space="preserve">purge CSS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Defer / async script cf screen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">balise canonical</t>
+  </si>
+  <si>
+    <t xml:space="preserve">parametrage cache</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CMS ou builder rapide</t>
+  </si>
+  <si>
+    <t xml:space="preserve">plugin de cache</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gzip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.htaccess</t>
   </si>
 </sst>
 </file>
@@ -309,6 +353,7 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -329,41 +374,48 @@
       <sz val="12"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF00A933"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -490,7 +542,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="1" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="2" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -570,10 +622,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z1004"/>
+  <dimension ref="A1:Z1005"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C62" activeCellId="0" sqref="C62"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A55" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A82" activeCellId="0" sqref="A82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.32421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -668,9 +720,6 @@
       <c r="E6" s="7"/>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="B7" s="1" t="s">
         <v>12</v>
       </c>
@@ -689,7 +738,7 @@
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E9" s="7"/>
@@ -698,7 +747,7 @@
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E10" s="7"/>
@@ -710,12 +759,6 @@
       <c r="B11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="E11" s="7"/>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -723,6 +766,12 @@
         <v>8</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>19</v>
       </c>
       <c r="E12" s="7"/>
@@ -732,48 +781,51 @@
         <v>8</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="E13" s="7"/>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="B14" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="E14" s="7"/>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B15" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>22</v>
       </c>
       <c r="E15" s="7"/>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="1" t="s">
         <v>23</v>
       </c>
       <c r="E16" s="7"/>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="8" t="s">
         <v>24</v>
       </c>
       <c r="E17" s="7"/>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B18" s="9" t="s">
+      <c r="B18" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="E18" s="7"/>
+    </row>
+    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B19" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="E18" s="7"/>
-    </row>
-    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B19" s="1" t="s">
+      <c r="C19" s="2" t="s">
         <v>27</v>
       </c>
       <c r="E19" s="7"/>
@@ -782,6 +834,7 @@
       <c r="B20" s="1" t="s">
         <v>28</v>
       </c>
+      <c r="E20" s="7"/>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B21" s="1" t="s">
@@ -789,21 +842,21 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B22" s="10" t="s">
+      <c r="B22" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B24" s="1" t="s">
+    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B23" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="D24" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
+    </row>
+    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B25" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D25" s="1" t="s">
         <v>33</v>
       </c>
     </row>
@@ -811,35 +864,35 @@
       <c r="B26" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C26" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D26" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>37</v>
-      </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B27" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D27" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="E27" s="1" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="1" t="s">
+      <c r="B28" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B28" s="1" t="s">
+    </row>
+    <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B30" s="1" t="s">
+      <c r="B29" s="1" t="s">
         <v>41</v>
       </c>
     </row>
+    <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B31" s="1" t="s">
         <v>42</v>
@@ -849,183 +902,234 @@
       <c r="B32" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C32" s="2" t="s">
+    </row>
+    <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B33" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+      <c r="C33" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B35" s="9" t="s">
+    <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B36" s="9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B36" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B37" s="12" t="s">
+      <c r="B37" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="48.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B38" s="1" t="s">
+    <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B38" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="C38" s="2" t="s">
+    </row>
+    <row r="39" customFormat="false" ht="48.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B39" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="40" customFormat="false" ht="26.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="41" customFormat="false" ht="25.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B41" s="1" t="s">
+      <c r="C39" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C41" s="13" t="s">
+    </row>
+    <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="41" customFormat="false" ht="26.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="42" customFormat="false" ht="25.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B42" s="1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B42" s="1" t="s">
+      <c r="C42" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="C42" s="2" t="s">
+    </row>
+    <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B43" s="1" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="43" customFormat="false" ht="32.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B43" s="1" t="s">
+      <c r="C43" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C43" s="13" t="s">
+    </row>
+    <row r="44" customFormat="false" ht="32.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B44" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="44" customFormat="false" ht="36.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B44" s="1" t="s">
+      <c r="C44" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="C44" s="13" t="s">
+    </row>
+    <row r="45" customFormat="false" ht="36.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B45" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="45" s="14" customFormat="true" ht="44.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B45" s="14" t="s">
+      <c r="C45" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="C45" s="15" t="s">
+    </row>
+    <row r="46" s="14" customFormat="true" ht="44.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B46" s="14" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C46" s="13"/>
-    </row>
-    <row r="47" s="14" customFormat="true" ht="47" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B47" s="14" t="s">
+      <c r="C46" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="C47" s="13" t="s">
+    </row>
+    <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C47" s="13"/>
+    </row>
+    <row r="48" s="14" customFormat="true" ht="47" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B48" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="F47" s="16"/>
-    </row>
-    <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B48" s="1" t="s">
+      <c r="C48" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="C48" s="2" t="s">
+      <c r="F48" s="16"/>
+    </row>
+    <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B49" s="1" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B50" s="1" t="s">
+      <c r="C49" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B52" s="1" t="s">
+    <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B51" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C52" s="2" t="s">
+    </row>
+    <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B53" s="1" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="54" s="14" customFormat="true" ht="47" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B54" s="14" t="s">
+      <c r="C53" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C54" s="13" t="s">
+    </row>
+    <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="55" s="14" customFormat="true" ht="47" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B55" s="14" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B56" s="1" t="s">
+      <c r="C55" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="C56" s="2" t="s">
+    </row>
+    <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B57" s="1" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B58" s="1" t="s">
+      <c r="C57" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C58" s="2" t="s">
+    </row>
+    <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B59" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="D58" s="17" t="s">
+      <c r="C59" s="2" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="60" s="14" customFormat="true" ht="36.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B60" s="14" t="s">
+      <c r="D59" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="C60" s="13" t="s">
+    </row>
+    <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="61" s="14" customFormat="true" ht="36.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B61" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="D60" s="14" t="s">
+      <c r="C61" s="13" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C61" s="2" t="s">
+      <c r="D61" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="D61" s="1" t="s">
+    </row>
+    <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C62" s="2" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+      <c r="D62" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B64" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
     <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C67" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
     <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B69" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B70" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B71" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
     <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B73" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
     <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B75" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
     <row r="76" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="77" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="77" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B77" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
     <row r="78" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="79" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="79" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B79" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
     <row r="80" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="81" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="82" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="81" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B81" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A82" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
     <row r="83" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="84" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="85" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1948,6 +2052,7 @@
     <row r="1002" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1003" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1004" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1005" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
not really making any progress.. trying to integrate with webpack on a side project. having weird errors
</commit_message>
<xml_diff>
--- a/report/Modèle-audit-SEO.xlsx
+++ b/report/Modèle-audit-SEO.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="92">
   <si>
     <t xml:space="preserve">Catégorie</t>
   </si>
@@ -316,7 +316,7 @@
     <t xml:space="preserve">purge CSS</t>
   </si>
   <si>
-    <t xml:space="preserve">Defer / async script cf screen</t>
+    <t xml:space="preserve">Defer / async script cf screen assets, critical files..</t>
   </si>
   <si>
     <t xml:space="preserve">balise canonical</t>
@@ -328,13 +328,19 @@
     <t xml:space="preserve">CMS ou builder rapide</t>
   </si>
   <si>
-    <t xml:space="preserve">plugin de cache</t>
+    <t xml:space="preserve">plugin de cache (not avalable for githu pages</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://webapps.stackexchange.com/questions/119286/caching-assets-in-website-served-from-github-pages</t>
   </si>
   <si>
     <t xml:space="preserve">gzip</t>
   </si>
   <si>
     <t xml:space="preserve">.htaccess</t>
+  </si>
+  <si>
+    <t xml:space="preserve">minify JS</t>
   </si>
 </sst>
 </file>
@@ -344,7 +350,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -414,6 +420,13 @@
       <family val="0"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -469,7 +482,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -540,6 +553,10 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="2" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -621,8 +638,8 @@
   </sheetPr>
   <dimension ref="A1:Z1005"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A58" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B83" activeCellId="0" sqref="B83"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A55" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B72" activeCellId="0" sqref="B72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.32421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1112,19 +1129,26 @@
       <c r="B79" s="1" t="s">
         <v>87</v>
       </c>
+      <c r="E79" s="18" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="80" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="81" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B81" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B82" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="83" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B83" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
     <row r="84" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="85" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="86" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -2048,6 +2072,9 @@
     <row r="1004" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1005" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E79" r:id="rId1" display="https://webapps.stackexchange.com/questions/119286/caching-assets-in-website-served-from-github-pages"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>